<commit_message>
Random matches in round robin
</commit_message>
<xml_diff>
--- a/tournament.xlsx
+++ b/tournament.xlsx
@@ -459,14 +459,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Always action zero</t>
+          <t>Random Player</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>4.38</v>
       </c>
       <c r="D2" t="n">
         <v>8</v>
@@ -475,17 +475,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Random Player</t>
+          <t>Forgiving Tit for Tat</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="C3" t="n">
-        <v>3.62</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
@@ -495,26 +495,26 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="C4" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Forgiving Tit for Tat</t>
+          <t>Grim Trigger</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C5" t="n">
-        <v>3.12</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
         <v>8</v>
@@ -523,17 +523,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Grim Trigger</t>
+          <t>Always action zero</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C6" t="n">
-        <v>3.12</v>
+        <v>3.25</v>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -584,10 +584,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>40.7</v>
+        <v>36</v>
       </c>
       <c r="C2" t="n">
-        <v>5.09</v>
+        <v>4.5</v>
       </c>
       <c r="D2" t="n">
         <v>8</v>
@@ -596,30 +596,30 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Forgiving Tit for Tat</t>
+          <t>Always action zero</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>37.8</v>
+        <v>71.59999999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>4.72</v>
+        <v>4.47</v>
       </c>
       <c r="D3" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Tit for Tat</t>
+          <t>Grim Trigger</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>35.8</v>
+        <v>35.2</v>
       </c>
       <c r="C4" t="n">
-        <v>4.47</v>
+        <v>4.4</v>
       </c>
       <c r="D4" t="n">
         <v>8</v>
@@ -628,33 +628,33 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Always action zero</t>
+          <t>Forgiving Tit for Tat</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>35.59999999999999</v>
+        <v>67.19999999999999</v>
       </c>
       <c r="C5" t="n">
-        <v>4.45</v>
+        <v>4.2</v>
       </c>
       <c r="D5" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Grim Trigger</t>
+          <t>Tit for Tat</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>32.8</v>
+        <v>67.19999999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>4.1</v>
+        <v>4.2</v>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>